<commit_message>
batch conversion update v1.1
</commit_message>
<xml_diff>
--- a/2312932_soil.xlsx
+++ b/2312932_soil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qliang\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwu\Documents\testing\github\EDD_GPRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BAB872-8346-498E-B95B-F6B8FA3D70CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB587B9E-D38F-4629-97DF-6ADBF9245FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34350" yWindow="-900" windowWidth="14865" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="2" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>PREPDATE</t>
   </si>
   <si>
-    <t>MATRIX</t>
-  </si>
-  <si>
     <t>TESTCODE</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>SW8081B</t>
+  </si>
+  <si>
+    <t>MATRIXNAME</t>
   </si>
 </sst>
 </file>
@@ -555,19 +555,19 @@
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD2748"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
@@ -613,271 +613,271 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" t="s">
         <v>43</v>
-      </c>
-      <c r="L2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="P3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" t="s">
         <v>43</v>
-      </c>
-      <c r="L3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB4" t="s">
         <v>43</v>
-      </c>
-      <c r="L4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" t="s">
-        <v>47</v>
-      </c>
-      <c r="T4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>